<commit_message>
Need to sort coordinates clockwise
</commit_message>
<xml_diff>
--- a/test_triangle.xlsx
+++ b/test_triangle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahaf/PycharmProjects/excel_to_kml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D17B5EDA-D463-8141-84E4-52EF005569D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9992218-8E0D-9942-A865-78667EDC23E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17580" xr2:uid="{ED8C8DCE-E8FF-014F-BB2E-7439F5CC8C22}"/>
+    <workbookView xWindow="1740" yWindow="1320" windowWidth="15120" windowHeight="17520" xr2:uid="{ED8C8DCE-E8FF-014F-BB2E-7439F5CC8C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,36 +380,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722AB446-FCB3-134D-A274-303472705827}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>334717</v>
+        <v>344607</v>
       </c>
       <c r="B1">
-        <v>313905</v>
+        <v>281842</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>331346</v>
+        <v>325140</v>
       </c>
       <c r="B2">
-        <v>322951</v>
+        <v>291722</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>324238</v>
+        <v>323035</v>
       </c>
       <c r="B3">
-        <v>334102</v>
+        <v>255341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>351548</v>
+      </c>
+      <c r="B4">
+        <v>301403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>